<commit_message>
Able to compute global satisfaction
</commit_message>
<xml_diff>
--- a/Analysis60.xlsx
+++ b/Analysis60.xlsx
@@ -26,304 +26,304 @@
     <t>Percentage Distribution</t>
   </si>
   <si>
-    <t>writing hawkish memos</t>
+    <t>playing the piano</t>
   </si>
   <si>
     <t>CS</t>
   </si>
   <si>
+    <t>1.33%</t>
+  </si>
+  <si>
+    <t>singing rock songs</t>
+  </si>
+  <si>
+    <t>0.67%</t>
+  </si>
+  <si>
+    <t>writing modern fiction</t>
+  </si>
+  <si>
+    <t>CS+DS</t>
+  </si>
+  <si>
+    <t>0.33%</t>
+  </si>
+  <si>
+    <t>fighting Carthaginians</t>
+  </si>
+  <si>
+    <t>following the money</t>
+  </si>
+  <si>
+    <t>1.17%</t>
+  </si>
+  <si>
+    <t>making money</t>
+  </si>
+  <si>
+    <t>DS</t>
+  </si>
+  <si>
+    <t>2.33%</t>
+  </si>
+  <si>
+    <t>moaning about men</t>
+  </si>
+  <si>
+    <t>1.00%</t>
+  </si>
+  <si>
+    <t>writing romantic poetry</t>
+  </si>
+  <si>
+    <t>0.50%</t>
+  </si>
+  <si>
+    <t>pioneering new technologies</t>
+  </si>
+  <si>
+    <t>0.83%</t>
+  </si>
+  <si>
+    <t>solving mysteries</t>
+  </si>
+  <si>
+    <t>looking after mother</t>
+  </si>
+  <si>
+    <t>2.17%</t>
+  </si>
+  <si>
+    <t>selling consumer goods</t>
+  </si>
+  <si>
+    <t>cross-dressing in women's clothes</t>
+  </si>
+  <si>
+    <t>2.50%</t>
+  </si>
+  <si>
+    <t>signing sports memorabilia</t>
+  </si>
+  <si>
+    <t>moaning about women</t>
+  </si>
+  <si>
     <t>2.00%</t>
   </si>
   <si>
-    <t>wielding political power</t>
-  </si>
-  <si>
-    <t>0.50%</t>
-  </si>
-  <si>
-    <t>tracking down fugitives</t>
-  </si>
-  <si>
-    <t>DS</t>
-  </si>
-  <si>
-    <t>solving crimes</t>
-  </si>
-  <si>
-    <t>1.00%</t>
-  </si>
-  <si>
-    <t>promoting Eastern philosophy</t>
-  </si>
-  <si>
-    <t>CS+DS</t>
-  </si>
-  <si>
-    <t>1.33%</t>
-  </si>
-  <si>
-    <t>promoting nerd culture</t>
-  </si>
-  <si>
-    <t>leading armies into battle</t>
-  </si>
-  <si>
-    <t>2.17%</t>
-  </si>
-  <si>
-    <t>developing new technologies</t>
-  </si>
-  <si>
-    <t>0.33%</t>
-  </si>
-  <si>
-    <t>promoting the Dark Side</t>
+    <t>writing modern poetry</t>
+  </si>
+  <si>
+    <t>ranting about liberals</t>
+  </si>
+  <si>
+    <t>promoting conservative values</t>
+  </si>
+  <si>
+    <t>painting self-portraits</t>
+  </si>
+  <si>
+    <t>1.50%</t>
+  </si>
+  <si>
+    <t>pushing the hardline</t>
+  </si>
+  <si>
+    <t>leaking state secrets</t>
+  </si>
+  <si>
+    <t>eating donuts</t>
+  </si>
+  <si>
+    <t>gossiping with galpals</t>
+  </si>
+  <si>
+    <t>1.83%</t>
+  </si>
+  <si>
+    <t>playing rock music</t>
+  </si>
+  <si>
+    <t>writing pop songs</t>
+  </si>
+  <si>
+    <t>guarding the galaxy</t>
+  </si>
+  <si>
+    <t>making condescending remarks</t>
+  </si>
+  <si>
+    <t>performing serious acting</t>
+  </si>
+  <si>
+    <t>monetizing celebrity status</t>
+  </si>
+  <si>
+    <t>writing serialized stories</t>
+  </si>
+  <si>
+    <t>suppressing minorities</t>
+  </si>
+  <si>
+    <t>1.67%</t>
+  </si>
+  <si>
+    <t>performing magic tricks</t>
+  </si>
+  <si>
+    <t>singing Hipbop songs</t>
+  </si>
+  <si>
+    <t>starring in romantic comedies</t>
+  </si>
+  <si>
+    <t>chasing after women</t>
+  </si>
+  <si>
+    <t>winning tennis tournaments</t>
+  </si>
+  <si>
+    <t>defending the weak</t>
+  </si>
+  <si>
+    <t>starring in action movies</t>
+  </si>
+  <si>
+    <t>telling bad jokes</t>
+  </si>
+  <si>
+    <t>complaining about capitalism</t>
+  </si>
+  <si>
+    <t>performing Web searches</t>
+  </si>
+  <si>
+    <t>promoting Objectivism</t>
+  </si>
+  <si>
+    <t>0.17%</t>
+  </si>
+  <si>
+    <t>writing cook books</t>
+  </si>
+  <si>
+    <t>preaching tolerance</t>
+  </si>
+  <si>
+    <t>selling fast food</t>
   </si>
   <si>
     <t>0.00%</t>
   </si>
   <si>
+    <t>doing stand-up</t>
+  </si>
+  <si>
+    <t>winning boxing matches</t>
+  </si>
+  <si>
+    <t>hiding from extremists</t>
+  </si>
+  <si>
+    <t>ranting about politics</t>
+  </si>
+  <si>
     <t>hosting a late night chat show</t>
   </si>
   <si>
-    <t>2.50%</t>
+    <t>directing movies</t>
+  </si>
+  <si>
+    <t>painting colorful pictures</t>
+  </si>
+  <si>
+    <t>carrying secret plans</t>
+  </si>
+  <si>
+    <t>womanizing</t>
+  </si>
+  <si>
+    <t>writing pot-boilers</t>
+  </si>
+  <si>
+    <t>smoking herb</t>
+  </si>
+  <si>
+    <t>chasing electronic ghosts</t>
+  </si>
+  <si>
+    <t>fencing stolen goods</t>
+  </si>
+  <si>
+    <t>2.67%</t>
+  </si>
+  <si>
+    <t>singing protest songs</t>
+  </si>
+  <si>
+    <t>pushing haute couture</t>
+  </si>
+  <si>
+    <t>writing political satires</t>
+  </si>
+  <si>
+    <t>writing comedy</t>
+  </si>
+  <si>
+    <t>making bad movies</t>
+  </si>
+  <si>
+    <t>feeding the poor</t>
+  </si>
+  <si>
+    <t>campaigning for social causes</t>
+  </si>
+  <si>
+    <t>building rocket ships</t>
+  </si>
+  <si>
+    <t>offering medical opinions</t>
+  </si>
+  <si>
+    <t>singing pop songs</t>
   </si>
   <si>
     <t>singing to teenagers</t>
   </si>
   <si>
-    <t>1.50%</t>
-  </si>
-  <si>
-    <t>singing melancholy songs</t>
-  </si>
-  <si>
-    <t>0.83%</t>
-  </si>
-  <si>
-    <t>pioneering new technologies</t>
-  </si>
-  <si>
-    <t>campaigning for social causes</t>
-  </si>
-  <si>
-    <t>starring in action movies</t>
-  </si>
-  <si>
-    <t>0.67%</t>
-  </si>
-  <si>
-    <t>interviewing politicians</t>
-  </si>
-  <si>
-    <t>running an empire</t>
-  </si>
-  <si>
-    <t>playing rock music</t>
-  </si>
-  <si>
-    <t>1.17%</t>
-  </si>
-  <si>
-    <t>making lewd remarks</t>
-  </si>
-  <si>
-    <t>escaping from handcuffs</t>
-  </si>
-  <si>
-    <t>interpreting evidence</t>
-  </si>
-  <si>
-    <t>0.17%</t>
-  </si>
-  <si>
-    <t>starring in Hollywood movies</t>
-  </si>
-  <si>
-    <t>cheating clients</t>
-  </si>
-  <si>
-    <t>following the money</t>
-  </si>
-  <si>
-    <t>writing cook books</t>
-  </si>
-  <si>
-    <t>running a large metropolitan city</t>
-  </si>
-  <si>
-    <t>1.83%</t>
-  </si>
-  <si>
-    <t>writing mystery stories</t>
-  </si>
-  <si>
-    <t>promoting Catholic values</t>
-  </si>
-  <si>
-    <t>campaigning for environmental causes</t>
-  </si>
-  <si>
-    <t>incurring debts</t>
-  </si>
-  <si>
-    <t>gyrating hips</t>
-  </si>
-  <si>
-    <t>monetizing celebrity status</t>
-  </si>
-  <si>
-    <t>bullying schoolkids</t>
-  </si>
-  <si>
-    <t>hosting anodyne game shows</t>
-  </si>
-  <si>
-    <t>singing jazz songs</t>
-  </si>
-  <si>
-    <t>making unauthorized sex tapes</t>
-  </si>
-  <si>
-    <t>womanizing</t>
-  </si>
-  <si>
-    <t>1.67%</t>
-  </si>
-  <si>
-    <t>investing money</t>
-  </si>
-  <si>
-    <t>promoting capitalism</t>
-  </si>
-  <si>
-    <t>fawning on the boss</t>
-  </si>
-  <si>
-    <t>singing rock songs</t>
-  </si>
-  <si>
-    <t>playing basketball</t>
-  </si>
-  <si>
-    <t>hunting monsters</t>
-  </si>
-  <si>
-    <t>devising evil schemes</t>
-  </si>
-  <si>
-    <t>carving magnificent statues</t>
-  </si>
-  <si>
-    <t>studying gorillas up close</t>
-  </si>
-  <si>
-    <t>riding a bicycle</t>
-  </si>
-  <si>
-    <t>evading mercenaries</t>
-  </si>
-  <si>
-    <t>convicting criminals</t>
-  </si>
-  <si>
-    <t>doing raunchy stage acts</t>
-  </si>
-  <si>
-    <t>causing mayhem</t>
-  </si>
-  <si>
-    <t>making cartoons</t>
-  </si>
-  <si>
-    <t>writing short stories</t>
-  </si>
-  <si>
-    <t>cooking dinners</t>
-  </si>
-  <si>
-    <t>fighting with swords</t>
-  </si>
-  <si>
-    <t>testing new technologies</t>
-  </si>
-  <si>
-    <t>undermining authority</t>
-  </si>
-  <si>
-    <t>studying magic</t>
-  </si>
-  <si>
-    <t>running a bureaucracy</t>
-  </si>
-  <si>
-    <t>2.33%</t>
-  </si>
-  <si>
-    <t>having meltdowns in public</t>
-  </si>
-  <si>
-    <t>performing kung-fu moves</t>
-  </si>
-  <si>
-    <t>postulating bizarre theories</t>
-  </si>
-  <si>
-    <t>flipping hamburgers</t>
-  </si>
-  <si>
-    <t>studying science</t>
-  </si>
-  <si>
-    <t>suppressing violent urges</t>
-  </si>
-  <si>
-    <t>winning swimming competitions</t>
-  </si>
-  <si>
-    <t>smuggling contraband</t>
-  </si>
-  <si>
-    <t>warning about totalitarianism</t>
-  </si>
-  <si>
-    <t>eluding hunters</t>
-  </si>
-  <si>
-    <t>nursing a messiah complex</t>
-  </si>
-  <si>
-    <t>winning tennis tournaments</t>
-  </si>
-  <si>
-    <t>singing torch songs</t>
-  </si>
-  <si>
-    <t>campaigning for the presidency</t>
+    <t>driving around America</t>
+  </si>
+  <si>
+    <t>jumping over buses on motorbikes</t>
+  </si>
+  <si>
+    <t>fighting for justice</t>
+  </si>
+  <si>
+    <t>promoting feminism</t>
+  </si>
+  <si>
+    <t>providing comic relief</t>
+  </si>
+  <si>
+    <t>over-acting</t>
   </si>
   <si>
     <t>climbing social ladders</t>
   </si>
   <si>
-    <t>instigating rebellion</t>
-  </si>
-  <si>
-    <t>biting opponents</t>
-  </si>
-  <si>
-    <t>singing country music</t>
-  </si>
-  <si>
-    <t>phoning home</t>
-  </si>
-  <si>
-    <t>designing computer systems</t>
-  </si>
-  <si>
-    <t>performing office chores</t>
-  </si>
-  <si>
-    <t>spying on girls</t>
+    <t>making propagandistic movies</t>
+  </si>
+  <si>
+    <t>brewing magican potions</t>
+  </si>
+  <si>
+    <t>directing action movies</t>
+  </si>
+  <si>
+    <t>selling chrystal meth</t>
   </si>
 </sst>
 </file>
@@ -381,7 +381,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="35.5625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="31.97265625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="9.69921875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="13.85546875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="28.9375" customWidth="true" bestFit="true"/>
@@ -409,7 +409,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>0.38142171924784907</v>
+        <v>0.3313969467653612</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -423,7 +423,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>0.18057681290280642</v>
+        <v>0.3176922485571153</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -437,24 +437,24 @@
         <v>10</v>
       </c>
       <c r="C4" t="n">
-        <v>0.13711802846929447</v>
+        <v>0.20826103448327724</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.3583871245600255</v>
+        <v>0.3822138181559788</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
@@ -462,83 +462,83 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.34046597654582517</v>
+      </c>
+      <c r="D6" t="s">
         <v>14</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.36203289090776847</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.39650936256302616</v>
+        <v>0.35942274573127464</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C8" t="n">
-        <v>0.39892322728347906</v>
+        <v>0.3517743622508807</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="n">
-        <v>0.09163032893503385</v>
+        <v>0.3869256210564802</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C10" t="n">
-        <v>0.03562412846183403</v>
+        <v>0.3422924885513677</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C11" t="n">
-        <v>0.39256756705348744</v>
+        <v>0.05719384430726333</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12">
@@ -546,10 +546,10 @@
         <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C12" t="n">
-        <v>0.3989174191514278</v>
+        <v>0.331100867901987</v>
       </c>
       <c r="D12" t="s">
         <v>26</v>
@@ -560,27 +560,27 @@
         <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C13" t="n">
-        <v>0.36294986075115815</v>
+        <v>0.372540084754141</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.3327734093018259</v>
+      </c>
+      <c r="D14" t="s">
         <v>29</v>
-      </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" t="n">
-        <v>0.3909944148385279</v>
-      </c>
-      <c r="D14" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="15">
@@ -588,13 +588,13 @@
         <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C15" t="n">
-        <v>0.38683920392395926</v>
+        <v>0.31878569029219794</v>
       </c>
       <c r="D15" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16">
@@ -602,10 +602,10 @@
         <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C16" t="n">
-        <v>0.27177746133622954</v>
+        <v>0.3244439111595342</v>
       </c>
       <c r="D16" t="s">
         <v>32</v>
@@ -613,363 +613,363 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>0.38234154759657735</v>
+        <v>0.029219370436407304</v>
       </c>
       <c r="D17" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C18" t="n">
-        <v>0.22646832011932105</v>
+        <v>0.28239630861443027</v>
       </c>
       <c r="D18" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
         <v>5</v>
       </c>
       <c r="C19" t="n">
-        <v>0.38058321580026366</v>
+        <v>0.2926353784898117</v>
       </c>
       <c r="D19" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C20" t="n">
-        <v>0.3607500072123489</v>
+        <v>0.3971578204444958</v>
       </c>
       <c r="D20" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B21" t="s">
         <v>5</v>
       </c>
       <c r="C21" t="n">
-        <v>0.29890576772674404</v>
+        <v>0.3317615794385373</v>
       </c>
       <c r="D21" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C22" t="n">
-        <v>0.067010135600322</v>
+        <v>0.24122830469020032</v>
       </c>
       <c r="D22" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C23" t="n">
-        <v>0.23641390326342546</v>
+        <v>0.35841706596581746</v>
       </c>
       <c r="D23" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C24" t="n">
-        <v>0.24215471820560297</v>
+        <v>0.3059013717773605</v>
       </c>
       <c r="D24" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B25" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C25" t="n">
-        <v>0.39629997850158166</v>
+        <v>0.39145331448849413</v>
       </c>
       <c r="D25" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
       </c>
       <c r="C26" t="n">
-        <v>0.3369560251412239</v>
+        <v>0.18544455711724048</v>
       </c>
       <c r="D26" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B27" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C27" t="n">
-        <v>0.3203978047909483</v>
+        <v>0.2851974460362429</v>
       </c>
       <c r="D27" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C28" t="n">
-        <v>0.11610648703621651</v>
+        <v>0.3384821292079457</v>
       </c>
       <c r="D28" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B29" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C29" t="n">
-        <v>0.19877788726787773</v>
+        <v>0.2484884933424086</v>
       </c>
       <c r="D29" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B30" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C30" t="n">
-        <v>0.3271010157473811</v>
+        <v>0.2841175506321908</v>
       </c>
       <c r="D30" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B31" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C31" t="n">
-        <v>0.37193706294185463</v>
+        <v>0.2802051148532822</v>
       </c>
       <c r="D31" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B32" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C32" t="n">
-        <v>0.1994364083542234</v>
+        <v>0.36670993561982945</v>
       </c>
       <c r="D32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B33" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C33" t="n">
-        <v>0.2686695646034928</v>
+        <v>0.38709500174114775</v>
       </c>
       <c r="D33" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B34" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C34" t="n">
-        <v>0.26222839321887237</v>
+        <v>0.34833774691928376</v>
       </c>
       <c r="D34" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B35" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C35" t="n">
-        <v>0.19812000763440268</v>
+        <v>0.3113609282889523</v>
       </c>
       <c r="D35" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B36" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C36" t="n">
-        <v>0.39890399933676357</v>
+        <v>0.397570032540338</v>
       </c>
       <c r="D36" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B37" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C37" t="n">
-        <v>0.2462620856067288</v>
+        <v>0.3766667454113721</v>
       </c>
       <c r="D37" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B38" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C38" t="n">
-        <v>0.39482691721771307</v>
+        <v>0.17653035184638527</v>
       </c>
       <c r="D38" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="B39" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C39" t="n">
-        <v>0.24104026869929404</v>
+        <v>0.38551420045577767</v>
       </c>
       <c r="D39" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B40" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C40" t="n">
-        <v>0.36683580556858963</v>
+        <v>0.3790621227831342</v>
       </c>
       <c r="D40" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B41" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C41" t="n">
-        <v>0.33621086458967087</v>
+        <v>0.1476730885064266</v>
       </c>
       <c r="D41" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B42" t="s">
         <v>10</v>
       </c>
       <c r="C42" t="n">
-        <v>0.394243841459758</v>
+        <v>0.39839921013602914</v>
       </c>
       <c r="D42" t="s">
         <v>6</v>
@@ -977,100 +977,100 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B43" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C43" t="n">
-        <v>0.2398402226917691</v>
+        <v>0.3652955737336626</v>
       </c>
       <c r="D43" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B44" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C44" t="n">
-        <v>0.3897832287026928</v>
+        <v>0.39075252884043815</v>
       </c>
       <c r="D44" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B45" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C45" t="n">
-        <v>0.39881182958149847</v>
+        <v>0.15246894977354825</v>
       </c>
       <c r="D45" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B46" t="s">
         <v>10</v>
       </c>
       <c r="C46" t="n">
-        <v>0.37600644426686863</v>
+        <v>0.2940322001734219</v>
       </c>
       <c r="D46" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B47" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C47" t="n">
-        <v>0.1817807330989482</v>
+        <v>0.3758974620364979</v>
       </c>
       <c r="D47" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="B48" t="s">
         <v>10</v>
       </c>
       <c r="C48" t="n">
-        <v>0.3917673955019822</v>
+        <v>0.32472528032836495</v>
       </c>
       <c r="D48" t="s">
-        <v>58</v>
+        <v>8</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
+        <v>66</v>
+      </c>
+      <c r="B49" t="s">
+        <v>16</v>
+      </c>
+      <c r="C49" t="n">
+        <v>0.015607986601214202</v>
+      </c>
+      <c r="D49" t="s">
         <v>67</v>
-      </c>
-      <c r="B49" t="s">
-        <v>14</v>
-      </c>
-      <c r="C49" t="n">
-        <v>0.20216886004865292</v>
-      </c>
-      <c r="D49" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="50">
@@ -1078,13 +1078,13 @@
         <v>68</v>
       </c>
       <c r="B50" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C50" t="n">
-        <v>0.12950161274147207</v>
+        <v>0.14522977062070327</v>
       </c>
       <c r="D50" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="51">
@@ -1095,66 +1095,66 @@
         <v>10</v>
       </c>
       <c r="C51" t="n">
-        <v>0.18373234245537162</v>
+        <v>0.03113583386035944</v>
       </c>
       <c r="D51" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>34</v>
+        <v>70</v>
       </c>
       <c r="B52" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C52" t="n">
-        <v>0.13088021959336116</v>
+        <v>0.39020479244365136</v>
       </c>
       <c r="D52" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="B53" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C53" t="n">
-        <v>0.37895698608863837</v>
+        <v>0.19190739481684266</v>
       </c>
       <c r="D53" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B54" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C54" t="n">
-        <v>0.018075187541506037</v>
+        <v>0.3130392309023581</v>
       </c>
       <c r="D54" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>71</v>
+        <v>24</v>
       </c>
       <c r="B55" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C55" t="n">
-        <v>0.06747111040008061</v>
+        <v>0.39891116787434144</v>
       </c>
       <c r="D55" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="56">
@@ -1165,10 +1165,10 @@
         <v>10</v>
       </c>
       <c r="C56" t="n">
-        <v>0.28497276756830603</v>
+        <v>0.17033364191824674</v>
       </c>
       <c r="D56" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
     <row r="57">
@@ -1176,13 +1176,13 @@
         <v>73</v>
       </c>
       <c r="B57" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C57" t="n">
-        <v>0.1733789848796418</v>
+        <v>0.1948892896553095</v>
       </c>
       <c r="D57" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
     </row>
     <row r="58">
@@ -1190,13 +1190,13 @@
         <v>74</v>
       </c>
       <c r="B58" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C58" t="n">
-        <v>0.08757559779418933</v>
+        <v>0.029606281138419007</v>
       </c>
       <c r="D58" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
     </row>
     <row r="59">
@@ -1204,13 +1204,13 @@
         <v>75</v>
       </c>
       <c r="B59" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C59" t="n">
-        <v>0.3471492677257574</v>
+        <v>0.25583899007261024</v>
       </c>
       <c r="D59" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="60">
@@ -1218,139 +1218,139 @@
         <v>76</v>
       </c>
       <c r="B60" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C60" t="n">
-        <v>0.3152238810313809</v>
+        <v>0.24554543135637485</v>
       </c>
       <c r="D60" t="s">
-        <v>58</v>
+        <v>23</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>30</v>
+        <v>77</v>
       </c>
       <c r="B61" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C61" t="n">
-        <v>0.14225306389776468</v>
+        <v>0.38400218489972215</v>
       </c>
       <c r="D61" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B62" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C62" t="n">
-        <v>0.3680248965952233</v>
+        <v>0.3911096730752892</v>
       </c>
       <c r="D62" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B63" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C63" t="n">
-        <v>0.35962897307352876</v>
+        <v>0.3463620584324378</v>
       </c>
       <c r="D63" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B64" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C64" t="n">
-        <v>0.35977410346597244</v>
+        <v>0.36952572016444085</v>
       </c>
       <c r="D64" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B65" t="s">
         <v>10</v>
       </c>
       <c r="C65" t="n">
-        <v>0.37740471489177413</v>
+        <v>0.39842831010942875</v>
       </c>
       <c r="D65" t="s">
-        <v>81</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B66" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C66" t="n">
-        <v>0.11942249562788786</v>
+        <v>0.3918333409092457</v>
       </c>
       <c r="D66" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B67" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C67" t="n">
-        <v>0.28591376446100014</v>
+        <v>0.23143086444352512</v>
       </c>
       <c r="D67" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B68" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C68" t="n">
-        <v>0.39114978580462134</v>
+        <v>0.3971579078009839</v>
       </c>
       <c r="D68" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="B69" t="s">
         <v>10</v>
       </c>
       <c r="C69" t="n">
-        <v>0.046295318797607385</v>
+        <v>0.1702614253837687</v>
       </c>
       <c r="D69" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="70">
@@ -1361,175 +1361,175 @@
         <v>10</v>
       </c>
       <c r="C70" t="n">
-        <v>0.06462692856753464</v>
+        <v>0.39058455132076525</v>
       </c>
       <c r="D70" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>25</v>
+        <v>87</v>
       </c>
       <c r="B71" t="s">
         <v>5</v>
       </c>
       <c r="C71" t="n">
-        <v>0.36099880265667084</v>
+        <v>0.2695427461904123</v>
       </c>
       <c r="D71" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B72" t="s">
         <v>10</v>
       </c>
       <c r="C72" t="n">
-        <v>0.39894173934376337</v>
+        <v>0.3050071722092969</v>
       </c>
       <c r="D72" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>83</v>
+        <v>35</v>
       </c>
       <c r="B73" t="s">
         <v>10</v>
       </c>
       <c r="C73" t="n">
-        <v>0.3159464362245141</v>
+        <v>0.39692685826385504</v>
       </c>
       <c r="D73" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="B74" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C74" t="n">
-        <v>0.05762839992324523</v>
+        <v>0.3810027697195528</v>
       </c>
       <c r="D74" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B75" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C75" t="n">
-        <v>0.11394913132440934</v>
+        <v>0.19137334121529495</v>
       </c>
       <c r="D75" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B76" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C76" t="n">
-        <v>0.3918248837854365</v>
+        <v>0.11844912496659665</v>
       </c>
       <c r="D76" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B77" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C77" t="n">
-        <v>0.3842162249842369</v>
+        <v>0.3507395333320461</v>
       </c>
       <c r="D77" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B78" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C78" t="n">
-        <v>0.33901414586938916</v>
+        <v>0.3479333614003518</v>
       </c>
       <c r="D78" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B79" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C79" t="n">
-        <v>0.198268298341954</v>
+        <v>0.39894226951235645</v>
       </c>
       <c r="D79" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B80" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C80" t="n">
-        <v>0.19271765310962277</v>
+        <v>0.39722283143572246</v>
       </c>
       <c r="D80" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B81" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C81" t="n">
-        <v>0.34026576744703346</v>
+        <v>0.3987922187077178</v>
       </c>
       <c r="D81" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B82" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C82" t="n">
-        <v>0.10003793281260928</v>
+        <v>0.3933417560770052</v>
       </c>
       <c r="D82" t="s">
         <v>32</v>
@@ -1537,128 +1537,128 @@
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B83" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C83" t="n">
-        <v>0.39135209102041874</v>
+        <v>0.14031380584924052</v>
       </c>
       <c r="D83" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B84" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C84" t="n">
-        <v>0.36730401472530644</v>
+        <v>0.373571088986913</v>
       </c>
       <c r="D84" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B85" t="s">
         <v>5</v>
       </c>
       <c r="C85" t="n">
-        <v>0.16820324099277</v>
+        <v>0.31779869381528325</v>
       </c>
       <c r="D85" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="B86" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C86" t="n">
-        <v>0.3880990863689567</v>
+        <v>0.024214601156275117</v>
       </c>
       <c r="D86" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B87" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C87" t="n">
-        <v>0.398238206143044</v>
+        <v>0.10629247465496204</v>
       </c>
       <c r="D87" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>65</v>
+        <v>102</v>
       </c>
       <c r="B88" t="s">
         <v>10</v>
       </c>
       <c r="C88" t="n">
-        <v>0.39886728293060375</v>
+        <v>0.39691452820713957</v>
       </c>
       <c r="D88" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C89" t="n">
-        <v>0.3398198840665538</v>
+        <v>0.07100343467230107</v>
       </c>
       <c r="D89" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B90" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C90" t="n">
-        <v>0.1441603937747287</v>
+        <v>0.18205108937068754</v>
       </c>
       <c r="D90" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>103</v>
+        <v>53</v>
       </c>
       <c r="B91" t="s">
         <v>10</v>
       </c>
       <c r="C91" t="n">
-        <v>0.3329976458184782</v>
+        <v>0.3731467183259985</v>
       </c>
       <c r="D91" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>